<commit_message>
Update VERA - Referentiedata - 2022-07-15.xlsx
puntenberekeningsoort toegevoegd
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2022-07-15.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2022-07-15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VERA\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F0F287-3ED1-4DA2-98EE-26E17A39736D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FBDC16-D267-4F62-B287-CAA5310B4C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13106" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="823" yWindow="2580" windowWidth="24694" windowHeight="15214" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VERA referentiedata" sheetId="14" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8662" uniqueCount="4343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8674" uniqueCount="4347">
   <si>
     <t>Referentiedatasoort</t>
   </si>
@@ -13228,6 +13228,18 @@
   </si>
   <si>
     <t>Overige ruimte; is de bovenste verdieping direct onder het dak van een gebouw met een vaste trap zoals gedefinieerd voor het bepalen van de woningwaardering. De term wordt vooral gebruikt bij gebouwen met een puntdak. De bovenste verdieping van een gebouw met plat dak wordt meestal geen zolder genoemd. Een ruimte mag als vertrek worden gezien indien deze een vast trap heeft, de vloer begaanbaar en het dak beschoten is. Zolders zonder vaste trap leggen we niet vast als vertrek. Indien een woning een zolder heeft met een vlizotrap kan dit in de advertentietekst worden gemeld.</t>
+  </si>
+  <si>
+    <t>PUNTENBEREKENINGSOORT</t>
+  </si>
+  <si>
+    <t>Maandelijkse herberekening</t>
+  </si>
+  <si>
+    <t>Koppelen inschrijving</t>
+  </si>
+  <si>
+    <t>Intrekken gebeurtenis of sanctie</t>
   </si>
 </sst>
 </file>
@@ -14019,8 +14031,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1385" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:K1385" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1390" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:K1390" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K1385">
     <sortCondition ref="A2:A1385"/>
     <sortCondition ref="D2:D1385"/>
@@ -14396,11 +14408,11 @@
   <sheetPr codeName="Blad1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K1385"/>
+  <dimension ref="A1:K1390"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1199" sqref="A1199"/>
+      <pane ySplit="1" topLeftCell="A1383" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1390" sqref="A1390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -45580,6 +45592,95 @@
       </c>
       <c r="J1385" s="13"/>
       <c r="K1385" s="13"/>
+    </row>
+    <row r="1386" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1386" s="10" t="s">
+        <v>4343</v>
+      </c>
+      <c r="B1386" s="10"/>
+      <c r="C1386" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1386" s="11" t="s">
+        <v>4050</v>
+      </c>
+      <c r="E1386" s="11"/>
+      <c r="F1386" s="11"/>
+      <c r="G1386" s="11"/>
+      <c r="H1386" s="10"/>
+      <c r="I1386" s="10"/>
+      <c r="J1386" s="10"/>
+      <c r="K1386" s="10"/>
+    </row>
+    <row r="1387" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1387" s="10" t="s">
+        <v>4343</v>
+      </c>
+      <c r="B1387" s="10"/>
+      <c r="C1387" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1387" s="11" t="s">
+        <v>4344</v>
+      </c>
+      <c r="E1387" s="11"/>
+      <c r="F1387" s="11"/>
+      <c r="G1387" s="11"/>
+      <c r="H1387" s="10"/>
+      <c r="I1387" s="10"/>
+      <c r="J1387" s="10"/>
+      <c r="K1387" s="10"/>
+    </row>
+    <row r="1388" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1388" s="10" t="s">
+        <v>4343</v>
+      </c>
+      <c r="B1388" s="10"/>
+      <c r="C1388" s="10" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D1388" s="11" t="s">
+        <v>4345</v>
+      </c>
+      <c r="E1388" s="11"/>
+      <c r="F1388" s="11"/>
+      <c r="G1388" s="11"/>
+      <c r="H1388" s="10"/>
+      <c r="I1388" s="10"/>
+      <c r="J1388" s="10"/>
+      <c r="K1388" s="10"/>
+    </row>
+    <row r="1389" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1389" s="10" t="s">
+        <v>4343</v>
+      </c>
+      <c r="B1389" s="10"/>
+      <c r="C1389" s="10" t="s">
+        <v>979</v>
+      </c>
+      <c r="D1389" s="11" t="s">
+        <v>4346</v>
+      </c>
+      <c r="E1389" s="11"/>
+      <c r="F1389" s="11"/>
+      <c r="G1389" s="11"/>
+      <c r="H1389" s="10"/>
+      <c r="I1389" s="10"/>
+      <c r="J1389" s="10"/>
+      <c r="K1389" s="10"/>
+    </row>
+    <row r="1390" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1390" s="10"/>
+      <c r="B1390" s="10"/>
+      <c r="C1390" s="10"/>
+      <c r="D1390" s="11"/>
+      <c r="E1390" s="11"/>
+      <c r="F1390" s="11"/>
+      <c r="G1390" s="11"/>
+      <c r="H1390" s="10"/>
+      <c r="I1390" s="10"/>
+      <c r="J1390" s="10"/>
+      <c r="K1390" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>